<commit_message>
adaptation du build par Gradle
</commit_message>
<xml_diff>
--- a/test-files/poi/XlsxHelperTestsOutput1.xlsx
+++ b/test-files/poi/XlsxHelperTestsOutput1.xlsx
@@ -63,7 +63,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,7 +108,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>22497.666993310184</v>
+        <v>22497.023174085647</v>
       </c>
       <c r="D2" t="n">
         <v>1.87</v>
@@ -152,7 +152,7 @@
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>6175.666993645833</v>
+        <v>6175.023174340277</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>1.72</v>

</xml_diff>